<commit_message>
updated build_exe.sh and example excel table
</commit_message>
<xml_diff>
--- a/examples/example_excel_file.xlsx
+++ b/examples/example_excel_file.xlsx
@@ -7,15 +7,15 @@
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="kat. A"/>
-    <sheet r:id="rId2" sheetId="2" name="kat. B"/>
+    <sheet r:id="rId1" sheetId="1" name="cat. A"/>
+    <sheet r:id="rId2" sheetId="2" name="cat. B"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
   <si>
     <t>Spalte1</t>
   </si>
@@ -44,43 +44,55 @@
     <t>Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Vorname </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alter </t>
+  </si>
+  <si>
+    <t>Kordel</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stadt </t>
+  </si>
+  <si>
+    <t>Test 4</t>
+  </si>
+  <si>
+    <t>Test Name 4</t>
+  </si>
+  <si>
+    <t>crua</t>
+  </si>
+  <si>
+    <t>Somewhere</t>
+  </si>
+  <si>
+    <t>Test 5</t>
+  </si>
+  <si>
+    <t>Test Name 5</t>
+  </si>
+  <si>
+    <t>Test Name 6</t>
+  </si>
+  <si>
+    <t>Test 7</t>
+  </si>
+  <si>
+    <t>Test Name 7</t>
+  </si>
+  <si>
+    <t>Test 8</t>
+  </si>
+  <si>
+    <t>Test Name 8</t>
+  </si>
+  <si>
     <t>Vorname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alter </t>
-  </si>
-  <si>
-    <t>Kordel</t>
-  </si>
-  <si>
-    <t>Land</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stadt </t>
-  </si>
-  <si>
-    <t>Test 4</t>
-  </si>
-  <si>
-    <t>Test Name 4</t>
-  </si>
-  <si>
-    <t>crua</t>
-  </si>
-  <si>
-    <t>Somewhere</t>
-  </si>
-  <si>
-    <t>Test 5</t>
-  </si>
-  <si>
-    <t>Test Name 5</t>
-  </si>
-  <si>
-    <t>Test 6</t>
-  </si>
-  <si>
-    <t>Test Name 6</t>
   </si>
   <si>
     <t>Alter</t>
@@ -115,19 +127,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -163,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -171,14 +177,8 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -523,13 +523,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="16.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="16.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="15.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -542,7 +542,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -563,32 +563,32 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="3">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2">
         <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -603,15 +603,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="3">
+        <v>32</v>
+      </c>
+      <c r="D4" s="2">
         <v>42</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -626,15 +626,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="3">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2">
         <v>42</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -666,16 +666,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="19.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -721,7 +721,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -731,7 +731,7 @@
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -744,7 +744,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -754,7 +754,7 @@
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>42</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -767,17 +767,15 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
         <v>42</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -790,47 +788,59 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3"/>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="2"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>

</xml_diff>